<commit_message>
Adding timeCutPoints as an attribute for all probability events (modelled either by Bernoulli distribution or logistic regression). Updated generatev2 for PSA so that input parameters are sampled for each time period for which they are required (as specified by timeCutPoints)
</commit_message>
<xml_diff>
--- a/input/DES_Input_Definitions.xlsx
+++ b/input/DES_Input_Definitions.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\uol.le.ac.uk\root\staff\home\m\ms1001\My Documents\AAA\AAA_DES_model\New folder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\uol.le.ac.uk\root\staff\home\m\ms1001\My Documents\AAA\AAA_DES_model\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,9 +15,6 @@
     <sheet name="Input Definitions" sheetId="1" r:id="rId1"/>
     <sheet name="Notes" sheetId="3" r:id="rId2"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId3"/>
-  </externalReferences>
   <definedNames>
     <definedName name="blah">#REF!</definedName>
     <definedName name="YearsNeeded">#REF!</definedName>
@@ -1449,29 +1446,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Main Data Items"/>
-      <sheetName val="Growth and Rupture Rates"/>
-      <sheetName val="AAA Size Distribution"/>
-      <sheetName val="Model Parameters"/>
-      <sheetName val="Other cause mortality"/>
-      <sheetName val="Notes"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1738,8 +1712,8 @@
   <dimension ref="A1:XET101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <pane ySplit="4" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>